<commit_message>
insert the getexcelurl and new routing - dutyupdate
</commit_message>
<xml_diff>
--- a/code/static/FB.xlsx
+++ b/code/static/FB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\09060.gary.wu\code\FlaskRESTfulAPI\code\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9076513B-9569-4621-85D0-F6089FD1B741}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB3C667-657F-4A32-98BD-D4AC2216AC6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27690" yWindow="5610" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26820" yWindow="6480" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step1 - Input Data" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>Personal Required Rate of Return</t>
   </si>
   <si>
-    <t>8.69%</t>
+    <t>8.72%</t>
   </si>
   <si>
     <t>Shares Outstanding (M)</t>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="H10" s="14">
         <f>G10*(1+B16)/(B15-B16)</f>
-        <v>679358.99513043882</v>
+        <v>676326.14247360651</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="F13" s="19">
         <f>ROUND((1+B15)^3,2)</f>
-        <v>1.28</v>
+        <v>1.29</v>
       </c>
       <c r="G13" s="19">
         <f>ROUND((1+B15)^4,2)</f>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="F14" s="14">
         <f>F10/F13</f>
-        <v>29714.813821616615</v>
+        <v>29484.466427650594</v>
       </c>
       <c r="G14" s="14">
         <f>G10/G13</f>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="H14" s="14">
         <f>H10/H13</f>
-        <v>485256.4250931706</v>
+        <v>483090.1017668618</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="B15" s="29" t="str">
         <f>'Step1 - Input Data'!B4</f>
-        <v>8.69%</v>
+        <v>8.72%</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="B17" s="14">
         <f>SUM(D14:H14)</f>
-        <v>597139.85879582027</v>
+        <v>594743.18807554548</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="B19" s="32">
         <f>B17/B18</f>
-        <v>248.80827449825844</v>
+        <v>247.80966169814394</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
start write DB to handover
</commit_message>
<xml_diff>
--- a/code/static/FB.xlsx
+++ b/code/static/FB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\09060.gary.wu\code\FlaskRESTfulAPI\code\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB3C667-657F-4A32-98BD-D4AC2216AC6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E4A4AE-E508-4D41-8FD2-2C655D40DA32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26820" yWindow="6480" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26400" yWindow="2400" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step1 - Input Data" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>Personal Required Rate of Return</t>
   </si>
   <si>
-    <t>8.72%</t>
+    <t>8.66%</t>
   </si>
   <si>
     <t>Shares Outstanding (M)</t>
@@ -135,7 +135,7 @@
     <t>Growth Rate</t>
   </si>
   <si>
-    <t>17.15%</t>
+    <t>17.0%</t>
   </si>
   <si>
     <t>Discounted Free Cash Flow Valuation</t>
@@ -1131,19 +1131,19 @@
       </c>
       <c r="E10" s="14">
         <f>E12*$C$4</f>
-        <v>32466.890048373258</v>
+        <v>30988.164209867169</v>
       </c>
       <c r="F10" s="14">
         <f>F12*$C$4</f>
-        <v>38034.961691669268</v>
+        <v>36256.152125544591</v>
       </c>
       <c r="G10" s="14">
         <f>G12*$C$4</f>
-        <v>44557.957621790549</v>
+        <v>42419.697986887164</v>
       </c>
       <c r="H10" s="14">
         <f>G10*(1+B16)/(B15-B16)</f>
-        <v>676326.14247360651</v>
+        <v>649671.05024962337</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1162,15 +1162,15 @@
         <v>68820</v>
       </c>
       <c r="E11" s="17">
-        <v>89800</v>
+        <v>85710</v>
       </c>
       <c r="F11" s="17">
         <f>E11*(1+$C$5)</f>
-        <v>105200.7</v>
+        <v>100280.7</v>
       </c>
       <c r="G11" s="17">
         <f>F11*(1+$C$5)</f>
-        <v>123242.62005</v>
+        <v>117328.41899999999</v>
       </c>
       <c r="H11" s="19"/>
     </row>
@@ -1192,15 +1192,15 @@
       </c>
       <c r="E12" s="21">
         <f>E11*$C$3</f>
-        <v>31858.666157587249</v>
+        <v>30407.64227579959</v>
       </c>
       <c r="F12" s="21">
         <f>F11*$C$3</f>
-        <v>37322.427403613459</v>
+        <v>35576.941462685521</v>
       </c>
       <c r="G12" s="21">
         <f>G11*$C$3</f>
-        <v>43723.223703333169</v>
+        <v>41625.021511342056</v>
       </c>
       <c r="H12" s="19"/>
     </row>
@@ -1220,15 +1220,15 @@
       </c>
       <c r="F13" s="19">
         <f>ROUND((1+B15)^3,2)</f>
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="G13" s="19">
         <f>ROUND((1+B15)^4,2)</f>
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="H13" s="19">
         <f>G13</f>
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1243,19 +1243,19 @@
       </c>
       <c r="E14" s="14">
         <f>E10/E13</f>
-        <v>27514.31360031632</v>
+        <v>26261.156110056923</v>
       </c>
       <c r="F14" s="14">
         <f>F10/F13</f>
-        <v>29484.466427650594</v>
+        <v>28325.118848081711</v>
       </c>
       <c r="G14" s="14">
         <f>G10/G13</f>
-        <v>31827.112586993251</v>
+        <v>30517.768335890047</v>
       </c>
       <c r="H14" s="14">
         <f>H10/H13</f>
-        <v>483090.1017668618</v>
+        <v>467389.24478390173</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="B15" s="29" t="str">
         <f>'Step1 - Input Data'!B4</f>
-        <v>8.72%</v>
+        <v>8.66%</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="B17" s="14">
         <f>SUM(D14:H14)</f>
-        <v>594743.18807554548</v>
+        <v>575320.48177165398</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="B19" s="32">
         <f>B17/B18</f>
-        <v>247.80966169814394</v>
+        <v>239.71686740485583</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>